<commit_message>
Update last opened cell to open on meta tab
</commit_message>
<xml_diff>
--- a/documentation/_static/360-giving-schema-titles-with-dei-extension-2024.xlsx
+++ b/documentation/_static/360-giving-schema-titles-with-dei-extension-2024.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="16"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Meta" sheetId="1" state="visible" r:id="rId2"/>
@@ -567,8 +567,12 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -595,79 +599,79 @@
   </sheetPr>
   <dimension ref="A1:A14"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A3" activeCellId="1" sqref="1:1 A3"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5234375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.53515625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="0" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="s">
+      <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="s">
+      <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="0" t="s">
+      <c r="A4" s="1" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="0" t="s">
+      <c r="A5" s="1" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="0" t="s">
+      <c r="A6" s="1" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="0" t="s">
+      <c r="A7" s="1" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="0" t="s">
+      <c r="A8" s="1" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="0" t="s">
+      <c r="A9" s="1" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="0" t="s">
+      <c r="A10" s="1" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="0" t="s">
+      <c r="A11" s="1" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="0" t="s">
+      <c r="A12" s="1" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="0" t="s">
+      <c r="A13" s="1" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="0" t="s">
+      <c r="A14" s="1" t="s">
         <v>13</v>
       </c>
     </row>
@@ -690,31 +694,31 @@
   <dimension ref="A1:G1"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="1:1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5234375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.53515625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="0" t="s">
+      <c r="A1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="0" t="s">
+      <c r="B1" s="1" t="s">
         <v>104</v>
       </c>
-      <c r="C1" s="0" t="s">
+      <c r="C1" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="D1" s="0" t="s">
+      <c r="D1" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="E1" s="0" t="s">
+      <c r="E1" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="F1" s="0" t="s">
+      <c r="F1" s="1" t="s">
         <v>105</v>
       </c>
-      <c r="G1" s="0" t="s">
+      <c r="G1" s="1" t="s">
         <v>106</v>
       </c>
     </row>
@@ -737,43 +741,43 @@
   <dimension ref="A1:K1"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D1" activeCellId="0" sqref="1:1"/>
+      <selection pane="topLeft" activeCell="D1" activeCellId="0" sqref="D1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5234375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.53515625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="0" t="s">
+      <c r="A1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="0" t="s">
+      <c r="B1" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="C1" s="0" t="s">
+      <c r="C1" s="1" t="s">
         <v>107</v>
       </c>
-      <c r="D1" s="0" t="s">
+      <c r="D1" s="1" t="s">
         <v>108</v>
       </c>
-      <c r="E1" s="0" t="s">
+      <c r="E1" s="1" t="s">
         <v>109</v>
       </c>
-      <c r="F1" s="0" t="s">
+      <c r="F1" s="1" t="s">
         <v>110</v>
       </c>
-      <c r="G1" s="0" t="s">
+      <c r="G1" s="1" t="s">
         <v>111</v>
       </c>
-      <c r="H1" s="0" t="s">
+      <c r="H1" s="1" t="s">
         <v>112</v>
       </c>
-      <c r="I1" s="0" t="s">
+      <c r="I1" s="1" t="s">
         <v>113</v>
       </c>
-      <c r="J1" s="0" t="s">
+      <c r="J1" s="1" t="s">
         <v>114</v>
       </c>
-      <c r="K1" s="0" t="s">
+      <c r="K1" s="1" t="s">
         <v>115</v>
       </c>
     </row>
@@ -796,67 +800,67 @@
   <dimension ref="A1:S1"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="1:1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5234375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.53515625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="0" t="s">
+      <c r="A1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="0" t="s">
+      <c r="B1" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="C1" s="0" t="s">
+      <c r="C1" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="D1" s="0" t="s">
+      <c r="D1" s="1" t="s">
         <v>116</v>
       </c>
-      <c r="E1" s="0" t="s">
+      <c r="E1" s="1" t="s">
         <v>117</v>
       </c>
-      <c r="F1" s="0" t="s">
+      <c r="F1" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="G1" s="0" t="s">
+      <c r="G1" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="H1" s="0" t="s">
+      <c r="H1" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="I1" s="0" t="s">
+      <c r="I1" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="J1" s="0" t="s">
+      <c r="J1" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="K1" s="0" t="s">
+      <c r="K1" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="L1" s="0" t="s">
+      <c r="L1" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="M1" s="0" t="s">
+      <c r="M1" s="1" t="s">
         <v>118</v>
       </c>
-      <c r="N1" s="0" t="s">
+      <c r="N1" s="1" t="s">
         <v>119</v>
       </c>
-      <c r="O1" s="0" t="s">
+      <c r="O1" s="1" t="s">
         <v>120</v>
       </c>
-      <c r="P1" s="0" t="s">
+      <c r="P1" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="Q1" s="0" t="s">
+      <c r="Q1" s="1" t="s">
         <v>121</v>
       </c>
-      <c r="R1" s="0" t="s">
+      <c r="R1" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="S1" s="0" t="s">
+      <c r="S1" s="1" t="s">
         <v>122</v>
       </c>
     </row>
@@ -879,31 +883,31 @@
   <dimension ref="A1:G1"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B1" activeCellId="0" sqref="1:1"/>
+      <selection pane="topLeft" activeCell="B1" activeCellId="0" sqref="B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5234375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.53515625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="0" t="s">
+      <c r="A1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="0" t="s">
+      <c r="B1" s="1" t="s">
         <v>123</v>
       </c>
-      <c r="C1" s="0" t="s">
+      <c r="C1" s="1" t="s">
         <v>124</v>
       </c>
-      <c r="D1" s="0" t="s">
+      <c r="D1" s="1" t="s">
         <v>125</v>
       </c>
-      <c r="E1" s="0" t="s">
+      <c r="E1" s="1" t="s">
         <v>126</v>
       </c>
-      <c r="F1" s="0" t="s">
+      <c r="F1" s="1" t="s">
         <v>127</v>
       </c>
-      <c r="G1" s="0" t="s">
+      <c r="G1" s="1" t="s">
         <v>128</v>
       </c>
     </row>
@@ -926,13 +930,13 @@
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="1:1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5234375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.53515625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="0" t="s">
+      <c r="A1" s="1" t="s">
         <v>5</v>
       </c>
     </row>
@@ -955,13 +959,13 @@
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="1:1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5234375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.53515625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="0" t="s">
+      <c r="A1" s="1" t="s">
         <v>5</v>
       </c>
     </row>
@@ -984,13 +988,13 @@
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="1:1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5234375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.53515625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="0" t="s">
+      <c r="A1" s="1" t="s">
         <v>5</v>
       </c>
     </row>
@@ -1012,83 +1016,83 @@
   </sheetPr>
   <dimension ref="A1:X1"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="1:1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A3" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
-    <row r="1" s="1" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="1" t="s">
+    <row r="1" s="2" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="2" t="s">
         <v>129</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="2" t="s">
         <v>130</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="2" t="s">
         <v>131</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="2" t="s">
         <v>132</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" s="2" t="s">
         <v>133</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="G1" s="2" t="s">
         <v>134</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="H1" s="2" t="s">
         <v>135</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="I1" s="2" t="s">
         <v>136</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="J1" s="2" t="s">
         <v>137</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="K1" s="2" t="s">
         <v>138</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="L1" s="2" t="s">
         <v>139</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="M1" s="2" t="s">
         <v>140</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="N1" s="2" t="s">
         <v>141</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="O1" s="2" t="s">
         <v>142</v>
       </c>
-      <c r="P1" s="1" t="s">
+      <c r="P1" s="2" t="s">
         <v>143</v>
       </c>
-      <c r="Q1" s="1" t="s">
+      <c r="Q1" s="2" t="s">
         <v>144</v>
       </c>
-      <c r="R1" s="1" t="s">
+      <c r="R1" s="2" t="s">
         <v>145</v>
       </c>
-      <c r="S1" s="1" t="s">
+      <c r="S1" s="2" t="s">
         <v>146</v>
       </c>
-      <c r="T1" s="1" t="s">
+      <c r="T1" s="2" t="s">
         <v>147</v>
       </c>
-      <c r="U1" s="1" t="s">
+      <c r="U1" s="2" t="s">
         <v>148</v>
       </c>
-      <c r="V1" s="1" t="s">
+      <c r="V1" s="2" t="s">
         <v>149</v>
       </c>
-      <c r="W1" s="1" t="s">
+      <c r="W1" s="2" t="s">
         <v>150</v>
       </c>
-      <c r="X1" s="1" t="s">
+      <c r="X1" s="2" t="s">
         <v>151</v>
       </c>
     </row>
@@ -1111,148 +1115,148 @@
   <dimension ref="A1:AT1"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E1" activeCellId="0" sqref="1:1"/>
+      <selection pane="topLeft" activeCell="E1" activeCellId="0" sqref="E1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5234375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.53515625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="0" t="s">
+      <c r="A1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="0" t="s">
+      <c r="B1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="0" t="s">
+      <c r="C1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="D1" s="0" t="s">
+      <c r="D1" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="E1" s="0" t="s">
+      <c r="E1" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="F1" s="0" t="s">
+      <c r="F1" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="G1" s="0" t="s">
+      <c r="G1" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="H1" s="0" t="s">
+      <c r="H1" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="I1" s="0" t="s">
+      <c r="I1" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="J1" s="0" t="s">
+      <c r="J1" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="K1" s="0" t="s">
+      <c r="K1" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="L1" s="0" t="s">
+      <c r="L1" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="M1" s="0" t="s">
+      <c r="M1" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="N1" s="0" t="s">
+      <c r="N1" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="O1" s="0" t="s">
+      <c r="O1" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="P1" s="0" t="s">
+      <c r="P1" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="Q1" s="0" t="s">
+      <c r="Q1" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="R1" s="0" t="s">
+      <c r="R1" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="S1" s="0" t="s">
+      <c r="S1" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="T1" s="0" t="s">
+      <c r="T1" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="U1" s="0" t="s">
+      <c r="U1" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="V1" s="0" t="s">
+      <c r="V1" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="W1" s="0" t="s">
+      <c r="W1" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="X1" s="0" t="s">
+      <c r="X1" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="Y1" s="0" t="s">
+      <c r="Y1" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="Z1" s="0" t="s">
+      <c r="Z1" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="AA1" s="0" t="s">
+      <c r="AA1" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="AB1" s="0" t="s">
+      <c r="AB1" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="AC1" s="0" t="s">
+      <c r="AC1" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="AD1" s="0" t="s">
+      <c r="AD1" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="AE1" s="0" t="s">
+      <c r="AE1" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="AF1" s="0" t="s">
+      <c r="AF1" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="AG1" s="0" t="s">
+      <c r="AG1" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="AH1" s="0" t="s">
+      <c r="AH1" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="AI1" s="0" t="s">
+      <c r="AI1" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="AJ1" s="0" t="s">
+      <c r="AJ1" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="AK1" s="0" t="s">
+      <c r="AK1" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="AL1" s="0" t="s">
+      <c r="AL1" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="AM1" s="0" t="s">
+      <c r="AM1" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="AN1" s="0" t="s">
+      <c r="AN1" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="AO1" s="0" t="s">
+      <c r="AO1" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="AP1" s="0" t="s">
+      <c r="AP1" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="AQ1" s="0" t="s">
+      <c r="AQ1" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="AR1" s="0" t="s">
+      <c r="AR1" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="AS1" s="0" t="s">
+      <c r="AS1" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="AT1" s="0" t="s">
+      <c r="AT1" s="1" t="s">
         <v>56</v>
       </c>
     </row>
@@ -1275,31 +1279,31 @@
   <dimension ref="A1:G1"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G1" activeCellId="0" sqref="1:1"/>
+      <selection pane="topLeft" activeCell="G1" activeCellId="0" sqref="G1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5234375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.53515625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="0" t="s">
+      <c r="A1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="0" t="s">
+      <c r="B1" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="C1" s="0" t="s">
+      <c r="C1" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="D1" s="0" t="s">
+      <c r="D1" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="E1" s="0" t="s">
+      <c r="E1" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="F1" s="0" t="s">
+      <c r="F1" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="G1" s="0" t="s">
+      <c r="G1" s="1" t="s">
         <v>62</v>
       </c>
     </row>
@@ -1322,40 +1326,40 @@
   <dimension ref="A1:J1"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="1:1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5234375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.53515625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="0" t="s">
+      <c r="A1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="0" t="s">
+      <c r="B1" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="C1" s="0" t="s">
+      <c r="C1" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="D1" s="0" t="s">
+      <c r="D1" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="E1" s="0" t="s">
+      <c r="E1" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="F1" s="0" t="s">
+      <c r="F1" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="G1" s="0" t="s">
+      <c r="G1" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="H1" s="0" t="s">
+      <c r="H1" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="I1" s="0" t="s">
+      <c r="I1" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="J1" s="0" t="s">
+      <c r="J1" s="1" t="s">
         <v>65</v>
       </c>
     </row>
@@ -1378,31 +1382,31 @@
   <dimension ref="A1:G1"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="1:1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5234375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.53515625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="0" t="s">
+      <c r="A1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="0" t="s">
+      <c r="B1" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="C1" s="0" t="s">
+      <c r="C1" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="D1" s="0" t="s">
+      <c r="D1" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="E1" s="0" t="s">
+      <c r="E1" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="F1" s="0" t="s">
+      <c r="F1" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="G1" s="0" t="s">
+      <c r="G1" s="1" t="s">
         <v>71</v>
       </c>
     </row>
@@ -1425,43 +1429,43 @@
   <dimension ref="A1:K1"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="1:1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5234375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.53515625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="0" t="s">
+      <c r="A1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="0" t="s">
+      <c r="B1" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="C1" s="0" t="s">
+      <c r="C1" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="D1" s="0" t="s">
+      <c r="D1" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="E1" s="0" t="s">
+      <c r="E1" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="F1" s="0" t="s">
+      <c r="F1" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="G1" s="0" t="s">
+      <c r="G1" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="H1" s="0" t="s">
+      <c r="H1" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="I1" s="0" t="s">
+      <c r="I1" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="J1" s="0" t="s">
+      <c r="J1" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="K1" s="0" t="s">
+      <c r="K1" s="1" t="s">
         <v>80</v>
       </c>
     </row>
@@ -1484,67 +1488,67 @@
   <dimension ref="A1:S1"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="1:1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5234375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.53515625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="0" t="s">
+      <c r="A1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="0" t="s">
+      <c r="B1" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="C1" s="0" t="s">
+      <c r="C1" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="D1" s="0" t="s">
+      <c r="D1" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="E1" s="0" t="s">
+      <c r="E1" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="F1" s="0" t="s">
+      <c r="F1" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="G1" s="0" t="s">
+      <c r="G1" s="1" t="s">
         <v>83</v>
       </c>
-      <c r="H1" s="0" t="s">
+      <c r="H1" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="I1" s="0" t="s">
+      <c r="I1" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="J1" s="0" t="s">
+      <c r="J1" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="K1" s="0" t="s">
+      <c r="K1" s="1" t="s">
         <v>87</v>
       </c>
-      <c r="L1" s="0" t="s">
+      <c r="L1" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="M1" s="0" t="s">
+      <c r="M1" s="1" t="s">
         <v>89</v>
       </c>
-      <c r="N1" s="0" t="s">
+      <c r="N1" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="O1" s="0" t="s">
+      <c r="O1" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="P1" s="0" t="s">
+      <c r="P1" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="Q1" s="0" t="s">
+      <c r="Q1" s="1" t="s">
         <v>93</v>
       </c>
-      <c r="R1" s="0" t="s">
+      <c r="R1" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="S1" s="0" t="s">
+      <c r="S1" s="1" t="s">
         <v>95</v>
       </c>
     </row>
@@ -1567,31 +1571,31 @@
   <dimension ref="A1:G1"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="1:1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5234375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.53515625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="0" t="s">
+      <c r="A1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="0" t="s">
+      <c r="B1" s="1" t="s">
         <v>96</v>
       </c>
-      <c r="C1" s="0" t="s">
+      <c r="C1" s="1" t="s">
         <v>97</v>
       </c>
-      <c r="D1" s="0" t="s">
+      <c r="D1" s="1" t="s">
         <v>98</v>
       </c>
-      <c r="E1" s="0" t="s">
+      <c r="E1" s="1" t="s">
         <v>99</v>
       </c>
-      <c r="F1" s="0" t="s">
+      <c r="F1" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="G1" s="0" t="s">
+      <c r="G1" s="1" t="s">
         <v>101</v>
       </c>
     </row>
@@ -1614,28 +1618,28 @@
   <dimension ref="A1:F1"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B1" activeCellId="0" sqref="1:1"/>
+      <selection pane="topLeft" activeCell="B1" activeCellId="0" sqref="B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5234375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.53515625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="0" t="s">
+      <c r="A1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="0" t="s">
+      <c r="B1" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="C1" s="0" t="s">
+      <c r="C1" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="D1" s="0" t="s">
+      <c r="D1" s="1" t="s">
         <v>102</v>
       </c>
-      <c r="E1" s="0" t="s">
+      <c r="E1" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="F1" s="0" t="s">
+      <c r="F1" s="1" t="s">
         <v>103</v>
       </c>
     </row>

</xml_diff>